<commit_message>
get routes working for users
</commit_message>
<xml_diff>
--- a/the_resources_/checkpoint4_user_stories.xlsx
+++ b/the_resources_/checkpoint4_user_stories.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vania\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vania\Desktop\WCS\checkpoint4\the_resources_\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6DEF9DF-D255-48FB-A897-45884F41BCEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3477872C-82DA-4F3F-8126-C054D4608AAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -91,7 +91,7 @@
     <t>Manage all users</t>
   </si>
   <si>
-    <t>Can all users, see last loggin from specific user, block and unblock</t>
+    <t>Can see all users, see last loggin from specific user, block and unblock</t>
   </si>
 </sst>
 </file>
@@ -616,7 +616,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C19" sqref="C19"/>
+      <selection pane="bottomRight" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>

</xml_diff>